<commit_message>
Add scripts, results, figures, supplementary figures
</commit_message>
<xml_diff>
--- a/tables/Supplementary Tables.xlsx
+++ b/tables/Supplementary Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aminosaurier/Downloads/GenomeBiology submission June 2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aminosaurier/Downloads/Micro-C paper submission 2024-25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4DA6F3-B6C3-A746-8EBE-DA832F0DF802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13E36B2-90AD-CD41-B5BB-2F4C4340914B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15860" xr2:uid="{4EB150EE-EB04-9841-AB04-5747774F122B}"/>
+    <workbookView xWindow="780" yWindow="900" windowWidth="27640" windowHeight="15860" activeTab="5" xr2:uid="{4EB150EE-EB04-9841-AB04-5747774F122B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1 Micro-C libraries" sheetId="1" r:id="rId1"/>
@@ -187,21 +187,6 @@
     <t>liftover-based approach</t>
   </si>
   <si>
-    <t>Group 1</t>
-  </si>
-  <si>
-    <t>Group 2</t>
-  </si>
-  <si>
-    <t>Group 3</t>
-  </si>
-  <si>
-    <t>Group 4</t>
-  </si>
-  <si>
-    <t>Group 5</t>
-  </si>
-  <si>
     <t>BLAST-based approach</t>
   </si>
   <si>
@@ -230,6 +215,21 @@
   </si>
   <si>
     <t>EDIT</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Moderately Conserved</t>
+  </si>
+  <si>
+    <t>Highly Conserved</t>
+  </si>
+  <si>
+    <t>Core</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A16256F-5F78-C74A-8BAC-479A47114E9A}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -720,7 +720,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>14</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1332,13 +1332,13 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1391,7 +1391,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1600,7 +1600,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1899,7 +1899,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -2035,7 +2035,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D21">
         <v>9</v>
@@ -2137,7 +2137,7 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -2341,7 +2341,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -2531,7 +2531,7 @@
         <v>33</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2708,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F32D6D-50EF-E140-8DD3-0D0304213552}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <v>643</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>438</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>221</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>98</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>24</v>
@@ -2766,12 +2766,12 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>338</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>487</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <v>380</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>173</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>46</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B14">
         <v>1424</v>

</xml_diff>